<commit_message>
testing clean code repo on laptop 01
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/energy_operator_feedback_v002.xlsx
+++ b/feedback_forms/current_versions/energy_operator_feedback_v002.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\one_drive\code\pycharm\feedback_portal\feedback_forms\current_versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D0D04D-19B3-49FB-B7CB-86A0DFBF0B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647A4790-77F7-4F18-979C-2136DECADB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4327" yWindow="2053" windowWidth="17413" windowHeight="11467" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
+    <workbookView xWindow="4667" yWindow="2393" windowWidth="17413" windowHeight="11467" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="5" r:id="rId1"/>
@@ -657,27 +657,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Q6.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Was an OGI inspection performed?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Q9.</t>
     </r>
     <r>
@@ -824,25 +803,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Q22. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Additional notes or comments.</t>
-    </r>
-  </si>
-  <si>
     <t>Q13 Answer.</t>
   </si>
   <si>
@@ -881,27 +841,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Q8.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> If you answered 'Yes' to Q6, what type of source was found using OGI?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Q10.</t>
     </r>
     <r>
@@ -912,27 +851,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">  If you answered 'Yes' to Q9, what date and time was the Method 21 inspection performed?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Q11.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> If you answered 'Yes' to Q9, what type of source was found using Method 21?</t>
     </r>
   </si>
   <si>
@@ -1128,6 +1046,88 @@
   <si>
     <t>energy_v00_01</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Q22.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Additional notes or comments.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Q11.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  If you answered 'Yes' to Q9, what type of source was found using Method 21?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Q6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Was an OGI inspection performed?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Q8.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  If you answered 'Yes' to Q6, what type of source was found using OGI?</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1136,13 +1136,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1405,10 +1411,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1418,8 +1424,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1430,8 +1436,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1443,45 +1449,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1489,94 +1501,91 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2688,9 +2697,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AG66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
@@ -2750,7 +2757,7 @@
     </row>
     <row r="3" spans="2:33" s="23" customFormat="1" ht="51" x14ac:dyDescent="0.5">
       <c r="B3" s="24" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -3025,7 +3032,7 @@
     </row>
     <row r="16" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B16" s="63" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
@@ -3664,8 +3671,8 @@
       </c>
     </row>
     <row r="44" spans="2:33" s="15" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44" s="59" t="s">
-        <v>162</v>
+      <c r="B44" s="64" t="s">
+        <v>210</v>
       </c>
       <c r="C44" s="41"/>
       <c r="D44" s="38" t="s">
@@ -3675,8 +3682,8 @@
       <c r="F44" s="41"/>
     </row>
     <row r="45" spans="2:33" s="15" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45" s="59" t="s">
-        <v>173</v>
+      <c r="B45" s="64" t="s">
+        <v>171</v>
       </c>
       <c r="C45" s="41"/>
       <c r="D45" s="50">
@@ -3686,8 +3693,8 @@
       <c r="F45" s="41"/>
     </row>
     <row r="46" spans="2:33" s="15" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" s="59" t="s">
-        <v>174</v>
+      <c r="B46" s="64" t="s">
+        <v>211</v>
       </c>
       <c r="C46" s="41"/>
       <c r="D46" s="38" t="s">
@@ -3698,7 +3705,7 @@
     </row>
     <row r="47" spans="2:33" s="15" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C47" s="41"/>
       <c r="D47" s="38" t="s">
@@ -3709,7 +3716,7 @@
     </row>
     <row r="48" spans="2:33" s="15" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="59" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C48" s="41"/>
       <c r="D48" s="50">
@@ -3719,8 +3726,8 @@
       <c r="F48" s="41"/>
     </row>
     <row r="49" spans="2:33" s="15" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="59" t="s">
-        <v>176</v>
+      <c r="B49" s="64" t="s">
+        <v>209</v>
       </c>
       <c r="C49" s="41"/>
       <c r="D49" s="38" t="s">
@@ -3731,7 +3738,7 @@
     </row>
     <row r="50" spans="2:33" s="15" customFormat="1" ht="30.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B50" s="59" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C50" s="41"/>
       <c r="D50" s="49">
@@ -3742,22 +3749,22 @@
     </row>
     <row r="51" spans="2:33" s="15" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
       <c r="B51" s="34" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C51" s="41"/>
       <c r="D51" s="60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E51" s="41"/>
       <c r="F51" s="41"/>
     </row>
     <row r="52" spans="2:33" s="15" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
       <c r="B52" s="59" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C52" s="41"/>
       <c r="D52" s="60" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E52" s="41"/>
       <c r="F52" s="41"/>
@@ -3870,7 +3877,7 @@
     </row>
     <row r="56" spans="2:33" s="15" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C56" s="34"/>
       <c r="D56" s="38" t="s">
@@ -3881,7 +3888,7 @@
     </row>
     <row r="57" spans="2:33" s="15" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="62" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C57" s="36"/>
       <c r="D57" s="60" t="s">
@@ -3892,7 +3899,7 @@
     </row>
     <row r="58" spans="2:33" s="15" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C58" s="34"/>
       <c r="D58" s="38" t="s">
@@ -3903,7 +3910,7 @@
     </row>
     <row r="59" spans="2:33" s="15" customFormat="1" ht="30.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B59" s="59" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C59" s="36"/>
       <c r="D59" s="60" t="s">
@@ -3914,7 +3921,7 @@
     </row>
     <row r="60" spans="2:33" s="15" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B60" s="59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C60" s="41"/>
       <c r="D60" s="50">
@@ -3925,7 +3932,7 @@
     </row>
     <row r="61" spans="2:33" s="15" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B61" s="59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C61" s="41"/>
       <c r="D61" s="49">
@@ -3936,11 +3943,11 @@
     </row>
     <row r="62" spans="2:33" s="15" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B62" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C62" s="34"/>
       <c r="D62" s="61" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E62" s="41"/>
       <c r="F62" s="41"/>
@@ -3986,11 +3993,11 @@
     </row>
     <row r="66" spans="2:6" s="15" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B66" s="34" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="C66" s="34"/>
       <c r="D66" s="60" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F66" s="41"/>
     </row>
@@ -4211,13 +4218,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D21" s="16">
         <v>45758</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F21" s="10" t="str">
         <f t="shared" ref="F21:F23" si="0">$B$16</f>
@@ -4230,20 +4237,20 @@
         <v>2</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D22" s="16">
         <v>45758</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F22" s="10" t="str">
         <f>$B$13</f>
         <v>Received</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="2:18" s="10" customFormat="1" ht="43" x14ac:dyDescent="0.5">
@@ -4251,13 +4258,13 @@
         <v>3</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D23" s="16">
         <v>45758</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F23" s="10" t="str">
         <f t="shared" si="0"/>
@@ -4270,20 +4277,20 @@
         <v>4</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D24" s="16">
         <v>45758</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F24" s="10" t="str">
         <f>$B$13</f>
         <v>Received</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
@@ -5780,7 +5787,7 @@
         <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -5982,7 +5989,7 @@
         <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D11" t="s">
         <v>91</v>
@@ -5991,7 +5998,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.5">
@@ -6033,7 +6040,7 @@
         <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D14" t="s">
         <v>94</v>
@@ -6050,7 +6057,7 @@
         <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D15" t="s">
         <v>95</v>
@@ -6067,7 +6074,7 @@
         <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D16" t="s">
         <v>96</v>
@@ -6084,7 +6091,7 @@
         <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D17" t="s">
         <v>97</v>
@@ -6101,7 +6108,7 @@
         <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D18" t="s">
         <v>98</v>
@@ -6118,7 +6125,7 @@
         <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D19" t="s">
         <v>99</v>
@@ -6169,7 +6176,7 @@
         <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D22" t="s">
         <v>103</v>
@@ -6203,7 +6210,7 @@
         <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D24" t="s">
         <v>105</v>
@@ -6237,7 +6244,7 @@
         <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D26" t="s">
         <v>108</v>
@@ -6246,7 +6253,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.5">
@@ -6254,7 +6261,7 @@
         <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D27" t="s">
         <v>109</v>
@@ -6271,7 +6278,7 @@
         <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D28" t="s">
         <v>110</v>
@@ -6288,7 +6295,7 @@
         <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D29" t="s">
         <v>131</v>
@@ -6305,7 +6312,7 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D30" t="s">
         <v>132</v>
@@ -6339,7 +6346,7 @@
         <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D32" t="s">
         <v>112</v>
@@ -6356,7 +6363,7 @@
         <v>77</v>
       </c>
       <c r="C33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D33" t="s">
         <v>135</v>
@@ -6373,7 +6380,7 @@
         <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D34" t="s">
         <v>136</v>
@@ -6390,7 +6397,7 @@
         <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D35" t="s">
         <v>137</v>
@@ -6416,7 +6423,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.5">
@@ -6441,7 +6448,7 @@
         <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D38" t="s">
         <v>116</v>
@@ -6450,7 +6457,7 @@
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -6463,6 +6470,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -6697,27 +6724,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368BC477-8FFD-4C56-8224-F3CCFEFBFA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{533C6BB5-3BBA-46E5-A63A-38A55F0F20F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6734,23 +6760,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368BC477-8FFD-4C56-8224-F3CCFEFBFA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>